<commit_message>
update api docs with new test cases
</commit_message>
<xml_diff>
--- a/Documents/1_TestCases/TC03_API/TC03_API_TestCase.xlsx
+++ b/Documents/1_TestCases/TC03_API/TC03_API_TestCase.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\Automation\OrangeHRM---Automation-Java-Playwright-JUnit-\Documents\1_TestCases\TC03_API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D694C6-9DAE-4939-BF8F-78F2E739619D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B08001-7425-41A8-AA36-8ED490CE29B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8115" yWindow="0" windowWidth="20685" windowHeight="15600" tabRatio="365" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Employees" sheetId="1" r:id="rId1"/>
+    <sheet name="Users" sheetId="2" r:id="rId2"/>
+    <sheet name="Projects" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="69">
   <si>
     <t>Test ID</t>
   </si>
@@ -76,13 +78,249 @@
   </si>
   <si>
     <t>/api/v2/pim/employees/</t>
+  </si>
+  <si>
+    <t>Auth token is available</t>
+  </si>
+  <si>
+    <t>Status 200</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>1.Generate a random user.
+2.Create the employee via ApiUtils.createEmployee() and get the employee Number.
+3.Build payload { "ids": [empNumber] }.
+4.Set headers:
+Content-Type: application/json
+Accept: application/json
+Cookie: _orangehrm={token}
+5.Send a DELETE request to /api/v2/pim/employees with the payload.
+6.Verify the response status is 200 OK.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Generate a random user using new User().generateRandomUser().
+ 2. Send a POST request using 
+ApiUtils.createEmployee() to create the employee and store the returned employee number.
+ 3. Verify that the returned employee number is greater than 0.
+ 4. Send a GET request to /api/v2/pim/employees/{employeeNumber}.
+Compare the response values with the original user data.</t>
+  </si>
+  <si>
+    <t>Values match</t>
+  </si>
+  <si>
+    <t>Requested user details match the created user details</t>
+  </si>
+  <si>
+    <t>API_TC03</t>
+  </si>
+  <si>
+    <t>Verify request to view employees details</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>1.Send a GET request using admin global user with empNumber "1" to /api/v2/pim/employees/{employeeNumber}
+2.Verify data match with admin user:
+firstName:admin
+middleName:middlename
+lastName:user
+employeeId:0001
+empNumber:1</t>
+  </si>
+  <si>
+    <t>Requested user details match the admin user details.</t>
+  </si>
+  <si>
+    <t>/api/v2/pim/employees/count</t>
+  </si>
+  <si>
+    <t>Verify employee count request is &gt;1</t>
+  </si>
+  <si>
+    <t>API_TC04</t>
+  </si>
+  <si>
+    <t>1. Add a random employee using the method from TC02.
+2.Send a GET request to endpoint.
+3.Verify response status is ok and larger than 1.</t>
+  </si>
+  <si>
+    <t>/api/v2/admin/users</t>
+  </si>
+  <si>
+    <t>API_USER_TC01</t>
+  </si>
+  <si>
+    <t>API_USER_TC02</t>
+  </si>
+  <si>
+    <t>API_USER_TC04</t>
+  </si>
+  <si>
+    <t>Verify request to create an user.</t>
+  </si>
+  <si>
+    <t>Verify request to retrive an user details.</t>
+  </si>
+  <si>
+    <t>Verify request to delete an user.</t>
+  </si>
+  <si>
+    <t>Verify request to uptate an user details.</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>/api/v2/admin/users/{id}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Use global admin user id:1
+2.Send a GET request to /api/v2/admin/users/{id}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status 200
+User role:Admin
+Emp name: admin user
+Status: enabled/true
+username: adminuser
+</t>
+  </si>
+  <si>
+    <t>User is present in the user list
+User can authenticate with created credentials.</t>
+  </si>
+  <si>
+    <t>1.Generate a new user
+2.Send a POST request to endpoint with following payload format:
+{
+  "status": true,
+  "username": "username",
+  "password": "password",
+  "userRoleId": 1
+}
+3.Verify user has been added and verify authentication with respective credentials</t>
+  </si>
+  <si>
+    <t>1.Generate and create a user as in test API_USER_TC02.
+2.Send a DELETE request to endpoint with following payload format:
+{
+  "ids": [&lt;int&gt;]
+}
+3.Verify user has been deleted.</t>
+  </si>
+  <si>
+    <t>User is no longer present in user list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Generate and create a user as in test API_USER_TC02
+2.Send a PUT request to endpoint with a payload format similar to API_USER_TC02 format and with updated data
+3.Verify if user details are updated.
+</t>
+  </si>
+  <si>
+    <t>User details have been updated accordingly</t>
+  </si>
+  <si>
+    <t>API_PROJECTS_TC01</t>
+  </si>
+  <si>
+    <t>API_PROJECTS_TC02</t>
+  </si>
+  <si>
+    <t>API_PROJECTS_TC03</t>
+  </si>
+  <si>
+    <t>API_PROJECTS_TC04</t>
+  </si>
+  <si>
+    <t>/api/v2/time/projects</t>
+  </si>
+  <si>
+    <t>Verify request to view a project details</t>
+  </si>
+  <si>
+    <t>Verify request to delete a project</t>
+  </si>
+  <si>
+    <t>Verify request to create a new project endpoint</t>
+  </si>
+  <si>
+    <t>Verify request to update a project</t>
+  </si>
+  <si>
+    <t>/api/v2/time/projects/{id}</t>
+  </si>
+  <si>
+    <t>1.Send a GET request to endpoint with {id} = 1
+2.Verify project details</t>
+  </si>
+  <si>
+    <t>Details should match:
+Name: Automation Project
+Description: Automation Project
+Customer Name: OrangeHRM
+Project Admin: Mary Great</t>
+  </si>
+  <si>
+    <t>Project details should match details added in the payload.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.Send a POST request to endpoint with the following payload format:
+{
+  "customerId": 1,
+  "name": "projectName",
+  "description": "projectDescription",
+  "projectAdminsEmpNumbers": [1]
+}
+2.Verify project request status and GET project details to confirm creation. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Response may not include details)</t>
+    </r>
+  </si>
+  <si>
+    <t>1.Send a DELETE request to endpoint with the following payload format:
+{
+  "ids": [1]
+}
+2.Verify request status.
+3.Send GET request to confirm project is not available anymore.</t>
+  </si>
+  <si>
+    <t>Delete request returns 200.
+Get request return 40X
+Project is not available.</t>
+  </si>
+  <si>
+    <t>1.Send a GET request to endpoint with {id} = 2 to retrieve info about project.
+2.Send a PUT request to endpoint with a format similar to API_PROJECTS_TC02 and with new data.
+3.Send a GET request to endpoint with {id} = 2 to retrieve info about project and cofirm the update has been succesfull.</t>
+  </si>
+  <si>
+    <t>Requests should return 200
+Project should update with the new data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +349,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -132,7 +384,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -149,11 +401,57 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="42">
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -173,7 +471,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -194,6 +492,88 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -236,7 +616,50 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -252,19 +675,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{7257DFA7-01A6-4206-A23E-FB97593526F5}" name="Table7" displayName="Table7" ref="B2:K498" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{7257DFA7-01A6-4206-A23E-FB97593526F5}" name="Table7" displayName="Table7" ref="B2:K498" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="B2:K498" xr:uid="{7257DFA7-01A6-4206-A23E-FB97593526F5}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{8A48E4F0-6353-4B65-A8AA-A9F47744DFE9}" name="Test ID" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{C69B3631-9235-49D5-835A-460725D8F78E}" name="Description/Title" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{80E1BC80-3B51-4B03-8EBD-561B4A7D6AD4}" name="Endpoint" dataDxfId="0"/>
-    <tableColumn id="11" xr3:uid="{27F69486-4DBB-4AA4-A6E5-9E4FCBF0452E}" name="Method" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{FE303652-83BF-4573-BA20-427DA11D17C1}" name="Preconditions" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{A40F81CC-1AF0-48A1-A33A-883B55562B5E}" name="Test Steps" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{8A0ED7D9-F5B9-4D05-BDCD-AA18270243C5}" name="Expected Result" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{95F71F64-2115-4AB0-9059-152D26C46054}" name="Actual Result" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{F94C22D6-3429-461D-B592-CC7FBFDC611E}" name="Notes" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{324B268D-5B58-47CB-AE05-5CFCA1EC0FCA}" name="Status" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{8A48E4F0-6353-4B65-A8AA-A9F47744DFE9}" name="Test ID" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{C69B3631-9235-49D5-835A-460725D8F78E}" name="Description/Title" dataDxfId="38"/>
+    <tableColumn id="9" xr3:uid="{80E1BC80-3B51-4B03-8EBD-561B4A7D6AD4}" name="Endpoint" dataDxfId="37"/>
+    <tableColumn id="11" xr3:uid="{27F69486-4DBB-4AA4-A6E5-9E4FCBF0452E}" name="Method" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{FE303652-83BF-4573-BA20-427DA11D17C1}" name="Preconditions" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{A40F81CC-1AF0-48A1-A33A-883B55562B5E}" name="Test Steps" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{8A0ED7D9-F5B9-4D05-BDCD-AA18270243C5}" name="Expected Result" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{95F71F64-2115-4AB0-9059-152D26C46054}" name="Actual Result" dataDxfId="32"/>
+    <tableColumn id="8" xr3:uid="{F94C22D6-3429-461D-B592-CC7FBFDC611E}" name="Notes" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{324B268D-5B58-47CB-AE05-5CFCA1EC0FCA}" name="Status" dataDxfId="30"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{30909C2A-1702-4CC2-8E90-B05A6262FD0C}" name="Table72" displayName="Table72" ref="B2:K498" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+  <autoFilter ref="B2:K498" xr:uid="{30909C2A-1702-4CC2-8E90-B05A6262FD0C}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{5245ECD6-3204-477A-8625-B349CD20F742}" name="Test ID" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{DE5092CA-7F23-4462-823F-F02DA362A4D0}" name="Description/Title" dataDxfId="26"/>
+    <tableColumn id="9" xr3:uid="{B3D237D4-EFE2-4271-B099-778174D53762}" name="Endpoint" dataDxfId="25"/>
+    <tableColumn id="11" xr3:uid="{D4FE0792-51A4-4606-9717-52FA7D6B5346}" name="Method" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{6600C647-C6D2-49E9-8165-9897BD96CCED}" name="Preconditions" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{244E144F-B53A-4AC8-9D48-FE790D597828}" name="Test Steps" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{DA2EF1E5-8819-4C9E-B458-B55805B50C09}" name="Expected Result" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{AF20225B-E0F2-4F44-8DC4-7C18A5D48316}" name="Actual Result" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{BA6833EF-7CCD-4BAA-B680-7D229DAE1464}" name="Notes" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{05780754-A8AB-493A-9863-C7D85E80A781}" name="Status" dataDxfId="18"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9C8EB052-938D-4D4D-B12E-C5AC8E21FC0E}" name="Table723" displayName="Table723" ref="B2:K498" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="B2:K498" xr:uid="{9C8EB052-938D-4D4D-B12E-C5AC8E21FC0E}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{8B447F5F-0218-44A8-9AD3-0BA2F0132139}" name="Test ID" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{D77FF6A0-CD02-4D99-8DEF-227253F4E9FC}" name="Description/Title" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{3B41C8A5-EB46-4059-8F73-33287EE9BE65}" name="Endpoint" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{B5E9853E-9C0B-477D-9161-7580076039E0}" name="Method" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{4D811123-D701-44EE-A284-D707FBE3753B}" name="Preconditions" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{489770C1-162F-420A-8DFC-5D079EA25964}" name="Test Steps" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{3D056CFF-89CB-412D-A5EB-A45D7A02B15B}" name="Expected Result" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{2765CC8E-9B99-450D-A70C-7EFAA02AF207}" name="Actual Result" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{C4579882-DBA1-426B-ABF8-139B3D94F8F2}" name="Notes" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{6F52D7A2-E330-4F92-AC74-2515DE0D07B1}" name="Status" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -535,8 +996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:K498"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,7 +1011,7 @@
     <col min="7" max="7" width="35.140625" style="3" customWidth="1"/>
     <col min="8" max="8" width="26.7109375" style="3" customWidth="1"/>
     <col min="9" max="9" width="33.7109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="48.5703125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="46.140625" style="3" customWidth="1"/>
     <col min="11" max="11" width="14.5703125" style="4" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
@@ -587,7 +1048,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
@@ -600,8 +1061,23 @@
       <c r="E3" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="F3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
@@ -614,12 +1090,67 @@
       <c r="E4" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D6" s="5"/>
+      <c r="F4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" s="5"/>
@@ -2100,10 +2631,10 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",K1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2121,4 +2652,3301 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F0733E0-18AD-4E8F-BD90-40A3BDD9A525}">
+  <dimension ref="B2:K498"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="35.140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="33.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="46.140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="5"/>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="5"/>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="5"/>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="5"/>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="5"/>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="5"/>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="5"/>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="5"/>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="5"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="5"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="5"/>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="5"/>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="5"/>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="5"/>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="5"/>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="5"/>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="5"/>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="5"/>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="5"/>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="5"/>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="5"/>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="5"/>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="5"/>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="5"/>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="5"/>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="5"/>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="5"/>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D51" s="5"/>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D52" s="5"/>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D53" s="5"/>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D54" s="5"/>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="5"/>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="5"/>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="5"/>
+    </row>
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="5"/>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="5"/>
+    </row>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D60" s="5"/>
+    </row>
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D61" s="5"/>
+    </row>
+    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D62" s="5"/>
+    </row>
+    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D63" s="5"/>
+    </row>
+    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D64" s="5"/>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="5"/>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D66" s="5"/>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D67" s="5"/>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D68" s="5"/>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D69" s="5"/>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D70" s="5"/>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D71" s="5"/>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D72" s="5"/>
+    </row>
+    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D73" s="5"/>
+    </row>
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D74" s="5"/>
+    </row>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D75" s="5"/>
+    </row>
+    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D76" s="5"/>
+    </row>
+    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D77" s="5"/>
+    </row>
+    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D78" s="5"/>
+    </row>
+    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D79" s="5"/>
+    </row>
+    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D80" s="5"/>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D81" s="5"/>
+    </row>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D82" s="5"/>
+    </row>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D83" s="5"/>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D84" s="5"/>
+    </row>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D85" s="5"/>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D86" s="5"/>
+    </row>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D87" s="5"/>
+    </row>
+    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D88" s="5"/>
+    </row>
+    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D89" s="5"/>
+    </row>
+    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D90" s="5"/>
+    </row>
+    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D91" s="5"/>
+    </row>
+    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D92" s="5"/>
+    </row>
+    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D93" s="5"/>
+    </row>
+    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D94" s="5"/>
+    </row>
+    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D95" s="5"/>
+    </row>
+    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D96" s="5"/>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D97" s="5"/>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D98" s="5"/>
+    </row>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D99" s="5"/>
+    </row>
+    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D100" s="5"/>
+    </row>
+    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D101" s="5"/>
+    </row>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D102" s="5"/>
+    </row>
+    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D103" s="5"/>
+    </row>
+    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D104" s="5"/>
+    </row>
+    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D105" s="5"/>
+    </row>
+    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D106" s="5"/>
+    </row>
+    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D107" s="5"/>
+    </row>
+    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D108" s="5"/>
+    </row>
+    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D109" s="5"/>
+    </row>
+    <row r="110" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D110" s="5"/>
+    </row>
+    <row r="111" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D111" s="5"/>
+    </row>
+    <row r="112" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D112" s="5"/>
+    </row>
+    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D113" s="5"/>
+    </row>
+    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D114" s="5"/>
+    </row>
+    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D115" s="5"/>
+    </row>
+    <row r="116" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D116" s="5"/>
+    </row>
+    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D117" s="5"/>
+    </row>
+    <row r="118" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D118" s="5"/>
+    </row>
+    <row r="119" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D119" s="5"/>
+    </row>
+    <row r="120" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D120" s="5"/>
+    </row>
+    <row r="121" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D121" s="5"/>
+    </row>
+    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D122" s="5"/>
+    </row>
+    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D123" s="5"/>
+    </row>
+    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D124" s="5"/>
+    </row>
+    <row r="125" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D125" s="5"/>
+    </row>
+    <row r="126" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D126" s="5"/>
+    </row>
+    <row r="127" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D127" s="5"/>
+    </row>
+    <row r="128" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D128" s="5"/>
+    </row>
+    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D129" s="5"/>
+    </row>
+    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D130" s="5"/>
+    </row>
+    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D131" s="5"/>
+    </row>
+    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D132" s="5"/>
+    </row>
+    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D133" s="5"/>
+    </row>
+    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D134" s="5"/>
+    </row>
+    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D135" s="5"/>
+    </row>
+    <row r="136" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D136" s="5"/>
+    </row>
+    <row r="137" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D137" s="5"/>
+    </row>
+    <row r="138" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D138" s="5"/>
+    </row>
+    <row r="139" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D139" s="5"/>
+    </row>
+    <row r="140" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D140" s="5"/>
+    </row>
+    <row r="141" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D141" s="5"/>
+    </row>
+    <row r="142" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D142" s="5"/>
+    </row>
+    <row r="143" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D143" s="5"/>
+    </row>
+    <row r="144" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D144" s="5"/>
+    </row>
+    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D145" s="5"/>
+    </row>
+    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D146" s="5"/>
+    </row>
+    <row r="147" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D147" s="5"/>
+    </row>
+    <row r="148" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D148" s="5"/>
+    </row>
+    <row r="149" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D149" s="5"/>
+    </row>
+    <row r="150" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D150" s="5"/>
+    </row>
+    <row r="151" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D151" s="5"/>
+    </row>
+    <row r="152" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D152" s="5"/>
+    </row>
+    <row r="153" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D153" s="5"/>
+    </row>
+    <row r="154" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D154" s="5"/>
+    </row>
+    <row r="155" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D155" s="5"/>
+    </row>
+    <row r="156" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D156" s="5"/>
+    </row>
+    <row r="157" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D157" s="5"/>
+    </row>
+    <row r="158" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D158" s="5"/>
+    </row>
+    <row r="159" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D159" s="5"/>
+    </row>
+    <row r="160" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D160" s="5"/>
+    </row>
+    <row r="161" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D161" s="5"/>
+    </row>
+    <row r="162" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D162" s="5"/>
+    </row>
+    <row r="163" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D163" s="5"/>
+    </row>
+    <row r="164" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D164" s="5"/>
+    </row>
+    <row r="165" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D165" s="5"/>
+    </row>
+    <row r="166" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D166" s="5"/>
+    </row>
+    <row r="167" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D167" s="5"/>
+    </row>
+    <row r="168" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D168" s="5"/>
+    </row>
+    <row r="169" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D169" s="5"/>
+    </row>
+    <row r="170" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D170" s="5"/>
+    </row>
+    <row r="171" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D171" s="5"/>
+    </row>
+    <row r="172" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D172" s="5"/>
+    </row>
+    <row r="173" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D173" s="5"/>
+    </row>
+    <row r="174" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D174" s="5"/>
+    </row>
+    <row r="175" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D175" s="5"/>
+    </row>
+    <row r="176" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D176" s="5"/>
+    </row>
+    <row r="177" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D177" s="5"/>
+    </row>
+    <row r="178" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D178" s="5"/>
+    </row>
+    <row r="179" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D179" s="5"/>
+    </row>
+    <row r="180" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D180" s="5"/>
+    </row>
+    <row r="181" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D181" s="5"/>
+    </row>
+    <row r="182" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D182" s="5"/>
+    </row>
+    <row r="183" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D183" s="5"/>
+    </row>
+    <row r="184" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D184" s="5"/>
+    </row>
+    <row r="185" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D185" s="5"/>
+    </row>
+    <row r="186" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D186" s="5"/>
+    </row>
+    <row r="187" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D187" s="5"/>
+    </row>
+    <row r="188" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D188" s="5"/>
+    </row>
+    <row r="189" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D189" s="5"/>
+    </row>
+    <row r="190" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D190" s="5"/>
+    </row>
+    <row r="191" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D191" s="5"/>
+    </row>
+    <row r="192" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D192" s="5"/>
+    </row>
+    <row r="193" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D193" s="5"/>
+    </row>
+    <row r="194" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D194" s="5"/>
+    </row>
+    <row r="195" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D195" s="5"/>
+    </row>
+    <row r="196" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D196" s="5"/>
+    </row>
+    <row r="197" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D197" s="5"/>
+    </row>
+    <row r="198" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D198" s="5"/>
+    </row>
+    <row r="199" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D199" s="5"/>
+    </row>
+    <row r="200" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D200" s="5"/>
+    </row>
+    <row r="201" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D201" s="5"/>
+    </row>
+    <row r="202" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D202" s="5"/>
+    </row>
+    <row r="203" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D203" s="5"/>
+    </row>
+    <row r="204" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D204" s="5"/>
+    </row>
+    <row r="205" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D205" s="5"/>
+    </row>
+    <row r="206" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D206" s="5"/>
+    </row>
+    <row r="207" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D207" s="5"/>
+    </row>
+    <row r="208" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D208" s="5"/>
+    </row>
+    <row r="209" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D209" s="5"/>
+    </row>
+    <row r="210" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D210" s="5"/>
+    </row>
+    <row r="211" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D211" s="5"/>
+    </row>
+    <row r="212" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D212" s="5"/>
+    </row>
+    <row r="213" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D213" s="5"/>
+    </row>
+    <row r="214" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D214" s="5"/>
+    </row>
+    <row r="215" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D215" s="5"/>
+    </row>
+    <row r="216" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D216" s="5"/>
+    </row>
+    <row r="217" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D217" s="5"/>
+    </row>
+    <row r="218" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D218" s="5"/>
+    </row>
+    <row r="219" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D219" s="5"/>
+    </row>
+    <row r="220" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D220" s="5"/>
+    </row>
+    <row r="221" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D221" s="5"/>
+    </row>
+    <row r="222" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D222" s="5"/>
+    </row>
+    <row r="223" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D223" s="5"/>
+    </row>
+    <row r="224" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D224" s="5"/>
+    </row>
+    <row r="225" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D225" s="5"/>
+    </row>
+    <row r="226" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D226" s="5"/>
+    </row>
+    <row r="227" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D227" s="5"/>
+    </row>
+    <row r="228" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D228" s="5"/>
+    </row>
+    <row r="229" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D229" s="5"/>
+    </row>
+    <row r="230" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D230" s="5"/>
+    </row>
+    <row r="231" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D231" s="5"/>
+    </row>
+    <row r="232" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D232" s="5"/>
+    </row>
+    <row r="233" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D233" s="5"/>
+    </row>
+    <row r="234" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D234" s="5"/>
+    </row>
+    <row r="235" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D235" s="5"/>
+    </row>
+    <row r="236" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D236" s="5"/>
+    </row>
+    <row r="237" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D237" s="5"/>
+    </row>
+    <row r="238" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D238" s="5"/>
+    </row>
+    <row r="239" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D239" s="5"/>
+    </row>
+    <row r="240" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D240" s="5"/>
+    </row>
+    <row r="241" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D241" s="5"/>
+    </row>
+    <row r="242" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D242" s="5"/>
+    </row>
+    <row r="243" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D243" s="5"/>
+    </row>
+    <row r="244" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D244" s="5"/>
+    </row>
+    <row r="245" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D245" s="5"/>
+    </row>
+    <row r="246" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D246" s="5"/>
+    </row>
+    <row r="247" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D247" s="5"/>
+    </row>
+    <row r="248" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D248" s="5"/>
+    </row>
+    <row r="249" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D249" s="5"/>
+    </row>
+    <row r="250" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D250" s="5"/>
+    </row>
+    <row r="251" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D251" s="5"/>
+    </row>
+    <row r="252" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D252" s="5"/>
+    </row>
+    <row r="253" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D253" s="5"/>
+    </row>
+    <row r="254" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D254" s="5"/>
+    </row>
+    <row r="255" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D255" s="5"/>
+    </row>
+    <row r="256" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D256" s="5"/>
+    </row>
+    <row r="257" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D257" s="5"/>
+    </row>
+    <row r="258" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D258" s="5"/>
+    </row>
+    <row r="259" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D259" s="5"/>
+    </row>
+    <row r="260" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D260" s="5"/>
+    </row>
+    <row r="261" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D261" s="5"/>
+    </row>
+    <row r="262" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D262" s="5"/>
+    </row>
+    <row r="263" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D263" s="5"/>
+    </row>
+    <row r="264" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D264" s="5"/>
+    </row>
+    <row r="265" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D265" s="5"/>
+    </row>
+    <row r="266" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D266" s="5"/>
+    </row>
+    <row r="267" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D267" s="5"/>
+    </row>
+    <row r="268" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D268" s="5"/>
+    </row>
+    <row r="269" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D269" s="5"/>
+    </row>
+    <row r="270" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D270" s="5"/>
+    </row>
+    <row r="271" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D271" s="5"/>
+    </row>
+    <row r="272" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D272" s="5"/>
+    </row>
+    <row r="273" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D273" s="5"/>
+    </row>
+    <row r="274" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D274" s="5"/>
+    </row>
+    <row r="275" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D275" s="5"/>
+    </row>
+    <row r="276" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D276" s="5"/>
+    </row>
+    <row r="277" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D277" s="5"/>
+    </row>
+    <row r="278" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D278" s="5"/>
+    </row>
+    <row r="279" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D279" s="5"/>
+    </row>
+    <row r="280" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D280" s="5"/>
+    </row>
+    <row r="281" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D281" s="5"/>
+    </row>
+    <row r="282" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D282" s="5"/>
+    </row>
+    <row r="283" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D283" s="5"/>
+    </row>
+    <row r="284" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D284" s="5"/>
+    </row>
+    <row r="285" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D285" s="5"/>
+    </row>
+    <row r="286" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D286" s="5"/>
+    </row>
+    <row r="287" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D287" s="5"/>
+    </row>
+    <row r="288" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D288" s="5"/>
+    </row>
+    <row r="289" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D289" s="5"/>
+    </row>
+    <row r="290" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D290" s="5"/>
+    </row>
+    <row r="291" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D291" s="5"/>
+    </row>
+    <row r="292" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D292" s="5"/>
+    </row>
+    <row r="293" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D293" s="5"/>
+    </row>
+    <row r="294" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D294" s="5"/>
+    </row>
+    <row r="295" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D295" s="5"/>
+    </row>
+    <row r="296" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D296" s="5"/>
+    </row>
+    <row r="297" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D297" s="5"/>
+    </row>
+    <row r="298" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D298" s="5"/>
+    </row>
+    <row r="299" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D299" s="5"/>
+    </row>
+    <row r="300" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D300" s="5"/>
+    </row>
+    <row r="301" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D301" s="5"/>
+    </row>
+    <row r="302" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D302" s="5"/>
+    </row>
+    <row r="303" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D303" s="5"/>
+    </row>
+    <row r="304" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D304" s="5"/>
+    </row>
+    <row r="305" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D305" s="5"/>
+    </row>
+    <row r="306" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D306" s="5"/>
+    </row>
+    <row r="307" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D307" s="5"/>
+    </row>
+    <row r="308" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D308" s="5"/>
+    </row>
+    <row r="309" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D309" s="5"/>
+    </row>
+    <row r="310" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D310" s="5"/>
+    </row>
+    <row r="311" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D311" s="5"/>
+    </row>
+    <row r="312" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D312" s="5"/>
+    </row>
+    <row r="313" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D313" s="5"/>
+    </row>
+    <row r="314" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D314" s="5"/>
+    </row>
+    <row r="315" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D315" s="5"/>
+    </row>
+    <row r="316" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D316" s="5"/>
+    </row>
+    <row r="317" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D317" s="5"/>
+    </row>
+    <row r="318" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D318" s="5"/>
+    </row>
+    <row r="319" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D319" s="5"/>
+    </row>
+    <row r="320" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D320" s="5"/>
+    </row>
+    <row r="321" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D321" s="5"/>
+    </row>
+    <row r="322" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D322" s="5"/>
+    </row>
+    <row r="323" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D323" s="5"/>
+    </row>
+    <row r="324" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D324" s="5"/>
+    </row>
+    <row r="325" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D325" s="5"/>
+    </row>
+    <row r="326" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D326" s="5"/>
+    </row>
+    <row r="327" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D327" s="5"/>
+    </row>
+    <row r="328" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D328" s="5"/>
+    </row>
+    <row r="329" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D329" s="5"/>
+    </row>
+    <row r="330" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D330" s="5"/>
+    </row>
+    <row r="331" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D331" s="5"/>
+    </row>
+    <row r="332" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D332" s="5"/>
+    </row>
+    <row r="333" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D333" s="5"/>
+    </row>
+    <row r="334" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D334" s="5"/>
+    </row>
+    <row r="335" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D335" s="5"/>
+    </row>
+    <row r="336" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D336" s="5"/>
+    </row>
+    <row r="337" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D337" s="5"/>
+    </row>
+    <row r="338" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D338" s="5"/>
+    </row>
+    <row r="339" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D339" s="5"/>
+    </row>
+    <row r="340" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D340" s="5"/>
+    </row>
+    <row r="341" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D341" s="5"/>
+    </row>
+    <row r="342" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D342" s="5"/>
+    </row>
+    <row r="343" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D343" s="5"/>
+    </row>
+    <row r="344" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D344" s="5"/>
+    </row>
+    <row r="345" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D345" s="5"/>
+    </row>
+    <row r="346" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D346" s="5"/>
+    </row>
+    <row r="347" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D347" s="5"/>
+    </row>
+    <row r="348" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D348" s="5"/>
+    </row>
+    <row r="349" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D349" s="5"/>
+    </row>
+    <row r="350" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D350" s="5"/>
+    </row>
+    <row r="351" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D351" s="5"/>
+    </row>
+    <row r="352" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D352" s="5"/>
+    </row>
+    <row r="353" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D353" s="5"/>
+    </row>
+    <row r="354" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D354" s="5"/>
+    </row>
+    <row r="355" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D355" s="5"/>
+    </row>
+    <row r="356" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D356" s="5"/>
+    </row>
+    <row r="357" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D357" s="5"/>
+    </row>
+    <row r="358" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D358" s="5"/>
+    </row>
+    <row r="359" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D359" s="5"/>
+    </row>
+    <row r="360" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D360" s="5"/>
+    </row>
+    <row r="361" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D361" s="5"/>
+    </row>
+    <row r="362" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D362" s="5"/>
+    </row>
+    <row r="363" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D363" s="5"/>
+    </row>
+    <row r="364" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D364" s="5"/>
+    </row>
+    <row r="365" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D365" s="5"/>
+    </row>
+    <row r="366" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D366" s="5"/>
+    </row>
+    <row r="367" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D367" s="5"/>
+    </row>
+    <row r="368" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D368" s="5"/>
+    </row>
+    <row r="369" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D369" s="5"/>
+    </row>
+    <row r="370" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D370" s="5"/>
+    </row>
+    <row r="371" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D371" s="5"/>
+    </row>
+    <row r="372" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D372" s="5"/>
+    </row>
+    <row r="373" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D373" s="5"/>
+    </row>
+    <row r="374" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D374" s="5"/>
+    </row>
+    <row r="375" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D375" s="5"/>
+    </row>
+    <row r="376" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D376" s="5"/>
+    </row>
+    <row r="377" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D377" s="5"/>
+    </row>
+    <row r="378" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D378" s="5"/>
+    </row>
+    <row r="379" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D379" s="5"/>
+    </row>
+    <row r="380" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D380" s="5"/>
+    </row>
+    <row r="381" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D381" s="5"/>
+    </row>
+    <row r="382" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D382" s="5"/>
+    </row>
+    <row r="383" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D383" s="5"/>
+    </row>
+    <row r="384" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D384" s="5"/>
+    </row>
+    <row r="385" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D385" s="5"/>
+    </row>
+    <row r="386" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D386" s="5"/>
+    </row>
+    <row r="387" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D387" s="5"/>
+    </row>
+    <row r="388" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D388" s="5"/>
+    </row>
+    <row r="389" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D389" s="5"/>
+    </row>
+    <row r="390" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D390" s="5"/>
+    </row>
+    <row r="391" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D391" s="5"/>
+    </row>
+    <row r="392" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D392" s="5"/>
+    </row>
+    <row r="393" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D393" s="5"/>
+    </row>
+    <row r="394" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D394" s="5"/>
+    </row>
+    <row r="395" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D395" s="5"/>
+    </row>
+    <row r="396" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D396" s="5"/>
+    </row>
+    <row r="397" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D397" s="5"/>
+    </row>
+    <row r="398" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D398" s="5"/>
+    </row>
+    <row r="399" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D399" s="5"/>
+    </row>
+    <row r="400" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D400" s="5"/>
+    </row>
+    <row r="401" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D401" s="5"/>
+    </row>
+    <row r="402" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D402" s="5"/>
+    </row>
+    <row r="403" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D403" s="5"/>
+    </row>
+    <row r="404" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D404" s="5"/>
+    </row>
+    <row r="405" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D405" s="5"/>
+    </row>
+    <row r="406" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D406" s="5"/>
+    </row>
+    <row r="407" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D407" s="5"/>
+    </row>
+    <row r="408" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D408" s="5"/>
+    </row>
+    <row r="409" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D409" s="5"/>
+    </row>
+    <row r="410" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D410" s="5"/>
+    </row>
+    <row r="411" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D411" s="5"/>
+    </row>
+    <row r="412" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D412" s="5"/>
+    </row>
+    <row r="413" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D413" s="5"/>
+    </row>
+    <row r="414" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D414" s="5"/>
+    </row>
+    <row r="415" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D415" s="5"/>
+    </row>
+    <row r="416" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D416" s="5"/>
+    </row>
+    <row r="417" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D417" s="5"/>
+    </row>
+    <row r="418" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D418" s="5"/>
+    </row>
+    <row r="419" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D419" s="5"/>
+    </row>
+    <row r="420" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D420" s="5"/>
+    </row>
+    <row r="421" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D421" s="5"/>
+    </row>
+    <row r="422" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D422" s="5"/>
+    </row>
+    <row r="423" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D423" s="5"/>
+    </row>
+    <row r="424" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D424" s="5"/>
+    </row>
+    <row r="425" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D425" s="5"/>
+    </row>
+    <row r="426" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D426" s="5"/>
+    </row>
+    <row r="427" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D427" s="5"/>
+    </row>
+    <row r="428" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D428" s="5"/>
+    </row>
+    <row r="429" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D429" s="5"/>
+    </row>
+    <row r="430" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D430" s="5"/>
+    </row>
+    <row r="431" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D431" s="5"/>
+    </row>
+    <row r="432" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D432" s="5"/>
+    </row>
+    <row r="433" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D433" s="5"/>
+    </row>
+    <row r="434" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D434" s="5"/>
+    </row>
+    <row r="435" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D435" s="5"/>
+    </row>
+    <row r="436" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D436" s="5"/>
+    </row>
+    <row r="437" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D437" s="5"/>
+    </row>
+    <row r="438" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D438" s="5"/>
+    </row>
+    <row r="439" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D439" s="5"/>
+    </row>
+    <row r="440" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D440" s="5"/>
+    </row>
+    <row r="441" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D441" s="5"/>
+    </row>
+    <row r="442" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D442" s="5"/>
+    </row>
+    <row r="443" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D443" s="5"/>
+    </row>
+    <row r="444" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D444" s="5"/>
+    </row>
+    <row r="445" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D445" s="5"/>
+    </row>
+    <row r="446" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D446" s="5"/>
+    </row>
+    <row r="447" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D447" s="5"/>
+    </row>
+    <row r="448" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D448" s="5"/>
+    </row>
+    <row r="449" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D449" s="5"/>
+    </row>
+    <row r="450" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D450" s="5"/>
+    </row>
+    <row r="451" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D451" s="5"/>
+    </row>
+    <row r="452" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D452" s="5"/>
+    </row>
+    <row r="453" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D453" s="5"/>
+    </row>
+    <row r="454" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D454" s="5"/>
+    </row>
+    <row r="455" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D455" s="5"/>
+    </row>
+    <row r="456" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D456" s="5"/>
+    </row>
+    <row r="457" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D457" s="5"/>
+    </row>
+    <row r="458" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D458" s="5"/>
+    </row>
+    <row r="459" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D459" s="5"/>
+    </row>
+    <row r="460" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D460" s="5"/>
+    </row>
+    <row r="461" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D461" s="5"/>
+    </row>
+    <row r="462" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D462" s="5"/>
+    </row>
+    <row r="463" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D463" s="5"/>
+    </row>
+    <row r="464" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D464" s="5"/>
+    </row>
+    <row r="465" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D465" s="5"/>
+    </row>
+    <row r="466" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D466" s="5"/>
+    </row>
+    <row r="467" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D467" s="5"/>
+    </row>
+    <row r="468" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D468" s="5"/>
+    </row>
+    <row r="469" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D469" s="5"/>
+    </row>
+    <row r="470" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D470" s="5"/>
+    </row>
+    <row r="471" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D471" s="5"/>
+    </row>
+    <row r="472" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D472" s="5"/>
+    </row>
+    <row r="473" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D473" s="5"/>
+    </row>
+    <row r="474" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D474" s="5"/>
+    </row>
+    <row r="475" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D475" s="5"/>
+    </row>
+    <row r="476" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D476" s="5"/>
+    </row>
+    <row r="477" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D477" s="5"/>
+    </row>
+    <row r="478" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D478" s="5"/>
+    </row>
+    <row r="479" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D479" s="5"/>
+    </row>
+    <row r="480" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D480" s="5"/>
+    </row>
+    <row r="481" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D481" s="5"/>
+    </row>
+    <row r="482" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D482" s="5"/>
+    </row>
+    <row r="483" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D483" s="5"/>
+    </row>
+    <row r="484" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D484" s="5"/>
+    </row>
+    <row r="485" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D485" s="5"/>
+    </row>
+    <row r="486" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D486" s="5"/>
+    </row>
+    <row r="487" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D487" s="5"/>
+    </row>
+    <row r="488" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D488" s="5"/>
+    </row>
+    <row r="489" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D489" s="5"/>
+    </row>
+    <row r="490" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D490" s="5"/>
+    </row>
+    <row r="491" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D491" s="5"/>
+    </row>
+    <row r="492" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D492" s="5"/>
+    </row>
+    <row r="493" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D493" s="5"/>
+    </row>
+    <row r="494" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D494" s="5"/>
+    </row>
+    <row r="495" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D495" s="5"/>
+    </row>
+    <row r="496" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D496" s="5"/>
+    </row>
+    <row r="497" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D497" s="5"/>
+    </row>
+    <row r="498" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D498" s="5"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="K1:K1048576">
+    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",K1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",K1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E498" xr:uid="{87AC3503-0EAF-4C8D-950F-A03BB57F756C}">
+      <formula1>"GET,POST,DELETE,PUT,HEAD,OPTION"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K498" xr:uid="{9DA21F42-E822-4190-B78A-3CEBE5B0E48D}">
+      <formula1>"Pass,Fail"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8267792D-E60E-4C51-8AAF-7230FC3414A8}">
+  <dimension ref="B2:K498"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="35.140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="29.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="33.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="46.140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="165" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="5"/>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="5"/>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="5"/>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="5"/>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="5"/>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="5"/>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="5"/>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="5"/>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="5"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="5"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="5"/>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="5"/>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="5"/>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="5"/>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="5"/>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="5"/>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="5"/>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="5"/>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="5"/>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="5"/>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="5"/>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="5"/>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="5"/>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="5"/>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="5"/>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="5"/>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="5"/>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D51" s="5"/>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D52" s="5"/>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D53" s="5"/>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D54" s="5"/>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="5"/>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="5"/>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="5"/>
+    </row>
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="5"/>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="5"/>
+    </row>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D60" s="5"/>
+    </row>
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D61" s="5"/>
+    </row>
+    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D62" s="5"/>
+    </row>
+    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D63" s="5"/>
+    </row>
+    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D64" s="5"/>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="5"/>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D66" s="5"/>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D67" s="5"/>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D68" s="5"/>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D69" s="5"/>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D70" s="5"/>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D71" s="5"/>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D72" s="5"/>
+    </row>
+    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D73" s="5"/>
+    </row>
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D74" s="5"/>
+    </row>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D75" s="5"/>
+    </row>
+    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D76" s="5"/>
+    </row>
+    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D77" s="5"/>
+    </row>
+    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D78" s="5"/>
+    </row>
+    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D79" s="5"/>
+    </row>
+    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D80" s="5"/>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D81" s="5"/>
+    </row>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D82" s="5"/>
+    </row>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D83" s="5"/>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D84" s="5"/>
+    </row>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D85" s="5"/>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D86" s="5"/>
+    </row>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D87" s="5"/>
+    </row>
+    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D88" s="5"/>
+    </row>
+    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D89" s="5"/>
+    </row>
+    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D90" s="5"/>
+    </row>
+    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D91" s="5"/>
+    </row>
+    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D92" s="5"/>
+    </row>
+    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D93" s="5"/>
+    </row>
+    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D94" s="5"/>
+    </row>
+    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D95" s="5"/>
+    </row>
+    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D96" s="5"/>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D97" s="5"/>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D98" s="5"/>
+    </row>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D99" s="5"/>
+    </row>
+    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D100" s="5"/>
+    </row>
+    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D101" s="5"/>
+    </row>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D102" s="5"/>
+    </row>
+    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D103" s="5"/>
+    </row>
+    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D104" s="5"/>
+    </row>
+    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D105" s="5"/>
+    </row>
+    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D106" s="5"/>
+    </row>
+    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D107" s="5"/>
+    </row>
+    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D108" s="5"/>
+    </row>
+    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D109" s="5"/>
+    </row>
+    <row r="110" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D110" s="5"/>
+    </row>
+    <row r="111" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D111" s="5"/>
+    </row>
+    <row r="112" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D112" s="5"/>
+    </row>
+    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D113" s="5"/>
+    </row>
+    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D114" s="5"/>
+    </row>
+    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D115" s="5"/>
+    </row>
+    <row r="116" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D116" s="5"/>
+    </row>
+    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D117" s="5"/>
+    </row>
+    <row r="118" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D118" s="5"/>
+    </row>
+    <row r="119" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D119" s="5"/>
+    </row>
+    <row r="120" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D120" s="5"/>
+    </row>
+    <row r="121" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D121" s="5"/>
+    </row>
+    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D122" s="5"/>
+    </row>
+    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D123" s="5"/>
+    </row>
+    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D124" s="5"/>
+    </row>
+    <row r="125" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D125" s="5"/>
+    </row>
+    <row r="126" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D126" s="5"/>
+    </row>
+    <row r="127" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D127" s="5"/>
+    </row>
+    <row r="128" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D128" s="5"/>
+    </row>
+    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D129" s="5"/>
+    </row>
+    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D130" s="5"/>
+    </row>
+    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D131" s="5"/>
+    </row>
+    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D132" s="5"/>
+    </row>
+    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D133" s="5"/>
+    </row>
+    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D134" s="5"/>
+    </row>
+    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D135" s="5"/>
+    </row>
+    <row r="136" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D136" s="5"/>
+    </row>
+    <row r="137" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D137" s="5"/>
+    </row>
+    <row r="138" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D138" s="5"/>
+    </row>
+    <row r="139" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D139" s="5"/>
+    </row>
+    <row r="140" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D140" s="5"/>
+    </row>
+    <row r="141" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D141" s="5"/>
+    </row>
+    <row r="142" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D142" s="5"/>
+    </row>
+    <row r="143" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D143" s="5"/>
+    </row>
+    <row r="144" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D144" s="5"/>
+    </row>
+    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D145" s="5"/>
+    </row>
+    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D146" s="5"/>
+    </row>
+    <row r="147" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D147" s="5"/>
+    </row>
+    <row r="148" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D148" s="5"/>
+    </row>
+    <row r="149" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D149" s="5"/>
+    </row>
+    <row r="150" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D150" s="5"/>
+    </row>
+    <row r="151" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D151" s="5"/>
+    </row>
+    <row r="152" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D152" s="5"/>
+    </row>
+    <row r="153" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D153" s="5"/>
+    </row>
+    <row r="154" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D154" s="5"/>
+    </row>
+    <row r="155" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D155" s="5"/>
+    </row>
+    <row r="156" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D156" s="5"/>
+    </row>
+    <row r="157" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D157" s="5"/>
+    </row>
+    <row r="158" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D158" s="5"/>
+    </row>
+    <row r="159" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D159" s="5"/>
+    </row>
+    <row r="160" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D160" s="5"/>
+    </row>
+    <row r="161" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D161" s="5"/>
+    </row>
+    <row r="162" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D162" s="5"/>
+    </row>
+    <row r="163" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D163" s="5"/>
+    </row>
+    <row r="164" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D164" s="5"/>
+    </row>
+    <row r="165" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D165" s="5"/>
+    </row>
+    <row r="166" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D166" s="5"/>
+    </row>
+    <row r="167" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D167" s="5"/>
+    </row>
+    <row r="168" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D168" s="5"/>
+    </row>
+    <row r="169" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D169" s="5"/>
+    </row>
+    <row r="170" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D170" s="5"/>
+    </row>
+    <row r="171" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D171" s="5"/>
+    </row>
+    <row r="172" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D172" s="5"/>
+    </row>
+    <row r="173" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D173" s="5"/>
+    </row>
+    <row r="174" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D174" s="5"/>
+    </row>
+    <row r="175" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D175" s="5"/>
+    </row>
+    <row r="176" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D176" s="5"/>
+    </row>
+    <row r="177" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D177" s="5"/>
+    </row>
+    <row r="178" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D178" s="5"/>
+    </row>
+    <row r="179" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D179" s="5"/>
+    </row>
+    <row r="180" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D180" s="5"/>
+    </row>
+    <row r="181" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D181" s="5"/>
+    </row>
+    <row r="182" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D182" s="5"/>
+    </row>
+    <row r="183" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D183" s="5"/>
+    </row>
+    <row r="184" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D184" s="5"/>
+    </row>
+    <row r="185" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D185" s="5"/>
+    </row>
+    <row r="186" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D186" s="5"/>
+    </row>
+    <row r="187" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D187" s="5"/>
+    </row>
+    <row r="188" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D188" s="5"/>
+    </row>
+    <row r="189" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D189" s="5"/>
+    </row>
+    <row r="190" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D190" s="5"/>
+    </row>
+    <row r="191" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D191" s="5"/>
+    </row>
+    <row r="192" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D192" s="5"/>
+    </row>
+    <row r="193" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D193" s="5"/>
+    </row>
+    <row r="194" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D194" s="5"/>
+    </row>
+    <row r="195" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D195" s="5"/>
+    </row>
+    <row r="196" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D196" s="5"/>
+    </row>
+    <row r="197" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D197" s="5"/>
+    </row>
+    <row r="198" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D198" s="5"/>
+    </row>
+    <row r="199" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D199" s="5"/>
+    </row>
+    <row r="200" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D200" s="5"/>
+    </row>
+    <row r="201" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D201" s="5"/>
+    </row>
+    <row r="202" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D202" s="5"/>
+    </row>
+    <row r="203" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D203" s="5"/>
+    </row>
+    <row r="204" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D204" s="5"/>
+    </row>
+    <row r="205" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D205" s="5"/>
+    </row>
+    <row r="206" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D206" s="5"/>
+    </row>
+    <row r="207" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D207" s="5"/>
+    </row>
+    <row r="208" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D208" s="5"/>
+    </row>
+    <row r="209" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D209" s="5"/>
+    </row>
+    <row r="210" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D210" s="5"/>
+    </row>
+    <row r="211" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D211" s="5"/>
+    </row>
+    <row r="212" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D212" s="5"/>
+    </row>
+    <row r="213" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D213" s="5"/>
+    </row>
+    <row r="214" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D214" s="5"/>
+    </row>
+    <row r="215" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D215" s="5"/>
+    </row>
+    <row r="216" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D216" s="5"/>
+    </row>
+    <row r="217" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D217" s="5"/>
+    </row>
+    <row r="218" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D218" s="5"/>
+    </row>
+    <row r="219" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D219" s="5"/>
+    </row>
+    <row r="220" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D220" s="5"/>
+    </row>
+    <row r="221" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D221" s="5"/>
+    </row>
+    <row r="222" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D222" s="5"/>
+    </row>
+    <row r="223" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D223" s="5"/>
+    </row>
+    <row r="224" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D224" s="5"/>
+    </row>
+    <row r="225" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D225" s="5"/>
+    </row>
+    <row r="226" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D226" s="5"/>
+    </row>
+    <row r="227" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D227" s="5"/>
+    </row>
+    <row r="228" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D228" s="5"/>
+    </row>
+    <row r="229" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D229" s="5"/>
+    </row>
+    <row r="230" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D230" s="5"/>
+    </row>
+    <row r="231" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D231" s="5"/>
+    </row>
+    <row r="232" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D232" s="5"/>
+    </row>
+    <row r="233" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D233" s="5"/>
+    </row>
+    <row r="234" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D234" s="5"/>
+    </row>
+    <row r="235" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D235" s="5"/>
+    </row>
+    <row r="236" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D236" s="5"/>
+    </row>
+    <row r="237" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D237" s="5"/>
+    </row>
+    <row r="238" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D238" s="5"/>
+    </row>
+    <row r="239" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D239" s="5"/>
+    </row>
+    <row r="240" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D240" s="5"/>
+    </row>
+    <row r="241" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D241" s="5"/>
+    </row>
+    <row r="242" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D242" s="5"/>
+    </row>
+    <row r="243" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D243" s="5"/>
+    </row>
+    <row r="244" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D244" s="5"/>
+    </row>
+    <row r="245" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D245" s="5"/>
+    </row>
+    <row r="246" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D246" s="5"/>
+    </row>
+    <row r="247" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D247" s="5"/>
+    </row>
+    <row r="248" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D248" s="5"/>
+    </row>
+    <row r="249" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D249" s="5"/>
+    </row>
+    <row r="250" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D250" s="5"/>
+    </row>
+    <row r="251" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D251" s="5"/>
+    </row>
+    <row r="252" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D252" s="5"/>
+    </row>
+    <row r="253" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D253" s="5"/>
+    </row>
+    <row r="254" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D254" s="5"/>
+    </row>
+    <row r="255" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D255" s="5"/>
+    </row>
+    <row r="256" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D256" s="5"/>
+    </row>
+    <row r="257" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D257" s="5"/>
+    </row>
+    <row r="258" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D258" s="5"/>
+    </row>
+    <row r="259" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D259" s="5"/>
+    </row>
+    <row r="260" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D260" s="5"/>
+    </row>
+    <row r="261" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D261" s="5"/>
+    </row>
+    <row r="262" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D262" s="5"/>
+    </row>
+    <row r="263" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D263" s="5"/>
+    </row>
+    <row r="264" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D264" s="5"/>
+    </row>
+    <row r="265" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D265" s="5"/>
+    </row>
+    <row r="266" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D266" s="5"/>
+    </row>
+    <row r="267" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D267" s="5"/>
+    </row>
+    <row r="268" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D268" s="5"/>
+    </row>
+    <row r="269" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D269" s="5"/>
+    </row>
+    <row r="270" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D270" s="5"/>
+    </row>
+    <row r="271" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D271" s="5"/>
+    </row>
+    <row r="272" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D272" s="5"/>
+    </row>
+    <row r="273" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D273" s="5"/>
+    </row>
+    <row r="274" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D274" s="5"/>
+    </row>
+    <row r="275" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D275" s="5"/>
+    </row>
+    <row r="276" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D276" s="5"/>
+    </row>
+    <row r="277" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D277" s="5"/>
+    </row>
+    <row r="278" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D278" s="5"/>
+    </row>
+    <row r="279" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D279" s="5"/>
+    </row>
+    <row r="280" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D280" s="5"/>
+    </row>
+    <row r="281" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D281" s="5"/>
+    </row>
+    <row r="282" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D282" s="5"/>
+    </row>
+    <row r="283" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D283" s="5"/>
+    </row>
+    <row r="284" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D284" s="5"/>
+    </row>
+    <row r="285" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D285" s="5"/>
+    </row>
+    <row r="286" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D286" s="5"/>
+    </row>
+    <row r="287" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D287" s="5"/>
+    </row>
+    <row r="288" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D288" s="5"/>
+    </row>
+    <row r="289" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D289" s="5"/>
+    </row>
+    <row r="290" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D290" s="5"/>
+    </row>
+    <row r="291" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D291" s="5"/>
+    </row>
+    <row r="292" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D292" s="5"/>
+    </row>
+    <row r="293" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D293" s="5"/>
+    </row>
+    <row r="294" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D294" s="5"/>
+    </row>
+    <row r="295" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D295" s="5"/>
+    </row>
+    <row r="296" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D296" s="5"/>
+    </row>
+    <row r="297" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D297" s="5"/>
+    </row>
+    <row r="298" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D298" s="5"/>
+    </row>
+    <row r="299" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D299" s="5"/>
+    </row>
+    <row r="300" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D300" s="5"/>
+    </row>
+    <row r="301" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D301" s="5"/>
+    </row>
+    <row r="302" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D302" s="5"/>
+    </row>
+    <row r="303" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D303" s="5"/>
+    </row>
+    <row r="304" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D304" s="5"/>
+    </row>
+    <row r="305" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D305" s="5"/>
+    </row>
+    <row r="306" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D306" s="5"/>
+    </row>
+    <row r="307" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D307" s="5"/>
+    </row>
+    <row r="308" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D308" s="5"/>
+    </row>
+    <row r="309" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D309" s="5"/>
+    </row>
+    <row r="310" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D310" s="5"/>
+    </row>
+    <row r="311" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D311" s="5"/>
+    </row>
+    <row r="312" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D312" s="5"/>
+    </row>
+    <row r="313" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D313" s="5"/>
+    </row>
+    <row r="314" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D314" s="5"/>
+    </row>
+    <row r="315" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D315" s="5"/>
+    </row>
+    <row r="316" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D316" s="5"/>
+    </row>
+    <row r="317" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D317" s="5"/>
+    </row>
+    <row r="318" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D318" s="5"/>
+    </row>
+    <row r="319" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D319" s="5"/>
+    </row>
+    <row r="320" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D320" s="5"/>
+    </row>
+    <row r="321" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D321" s="5"/>
+    </row>
+    <row r="322" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D322" s="5"/>
+    </row>
+    <row r="323" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D323" s="5"/>
+    </row>
+    <row r="324" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D324" s="5"/>
+    </row>
+    <row r="325" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D325" s="5"/>
+    </row>
+    <row r="326" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D326" s="5"/>
+    </row>
+    <row r="327" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D327" s="5"/>
+    </row>
+    <row r="328" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D328" s="5"/>
+    </row>
+    <row r="329" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D329" s="5"/>
+    </row>
+    <row r="330" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D330" s="5"/>
+    </row>
+    <row r="331" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D331" s="5"/>
+    </row>
+    <row r="332" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D332" s="5"/>
+    </row>
+    <row r="333" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D333" s="5"/>
+    </row>
+    <row r="334" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D334" s="5"/>
+    </row>
+    <row r="335" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D335" s="5"/>
+    </row>
+    <row r="336" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D336" s="5"/>
+    </row>
+    <row r="337" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D337" s="5"/>
+    </row>
+    <row r="338" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D338" s="5"/>
+    </row>
+    <row r="339" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D339" s="5"/>
+    </row>
+    <row r="340" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D340" s="5"/>
+    </row>
+    <row r="341" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D341" s="5"/>
+    </row>
+    <row r="342" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D342" s="5"/>
+    </row>
+    <row r="343" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D343" s="5"/>
+    </row>
+    <row r="344" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D344" s="5"/>
+    </row>
+    <row r="345" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D345" s="5"/>
+    </row>
+    <row r="346" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D346" s="5"/>
+    </row>
+    <row r="347" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D347" s="5"/>
+    </row>
+    <row r="348" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D348" s="5"/>
+    </row>
+    <row r="349" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D349" s="5"/>
+    </row>
+    <row r="350" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D350" s="5"/>
+    </row>
+    <row r="351" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D351" s="5"/>
+    </row>
+    <row r="352" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D352" s="5"/>
+    </row>
+    <row r="353" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D353" s="5"/>
+    </row>
+    <row r="354" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D354" s="5"/>
+    </row>
+    <row r="355" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D355" s="5"/>
+    </row>
+    <row r="356" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D356" s="5"/>
+    </row>
+    <row r="357" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D357" s="5"/>
+    </row>
+    <row r="358" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D358" s="5"/>
+    </row>
+    <row r="359" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D359" s="5"/>
+    </row>
+    <row r="360" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D360" s="5"/>
+    </row>
+    <row r="361" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D361" s="5"/>
+    </row>
+    <row r="362" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D362" s="5"/>
+    </row>
+    <row r="363" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D363" s="5"/>
+    </row>
+    <row r="364" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D364" s="5"/>
+    </row>
+    <row r="365" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D365" s="5"/>
+    </row>
+    <row r="366" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D366" s="5"/>
+    </row>
+    <row r="367" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D367" s="5"/>
+    </row>
+    <row r="368" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D368" s="5"/>
+    </row>
+    <row r="369" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D369" s="5"/>
+    </row>
+    <row r="370" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D370" s="5"/>
+    </row>
+    <row r="371" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D371" s="5"/>
+    </row>
+    <row r="372" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D372" s="5"/>
+    </row>
+    <row r="373" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D373" s="5"/>
+    </row>
+    <row r="374" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D374" s="5"/>
+    </row>
+    <row r="375" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D375" s="5"/>
+    </row>
+    <row r="376" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D376" s="5"/>
+    </row>
+    <row r="377" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D377" s="5"/>
+    </row>
+    <row r="378" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D378" s="5"/>
+    </row>
+    <row r="379" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D379" s="5"/>
+    </row>
+    <row r="380" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D380" s="5"/>
+    </row>
+    <row r="381" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D381" s="5"/>
+    </row>
+    <row r="382" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D382" s="5"/>
+    </row>
+    <row r="383" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D383" s="5"/>
+    </row>
+    <row r="384" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D384" s="5"/>
+    </row>
+    <row r="385" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D385" s="5"/>
+    </row>
+    <row r="386" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D386" s="5"/>
+    </row>
+    <row r="387" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D387" s="5"/>
+    </row>
+    <row r="388" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D388" s="5"/>
+    </row>
+    <row r="389" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D389" s="5"/>
+    </row>
+    <row r="390" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D390" s="5"/>
+    </row>
+    <row r="391" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D391" s="5"/>
+    </row>
+    <row r="392" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D392" s="5"/>
+    </row>
+    <row r="393" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D393" s="5"/>
+    </row>
+    <row r="394" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D394" s="5"/>
+    </row>
+    <row r="395" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D395" s="5"/>
+    </row>
+    <row r="396" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D396" s="5"/>
+    </row>
+    <row r="397" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D397" s="5"/>
+    </row>
+    <row r="398" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D398" s="5"/>
+    </row>
+    <row r="399" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D399" s="5"/>
+    </row>
+    <row r="400" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D400" s="5"/>
+    </row>
+    <row r="401" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D401" s="5"/>
+    </row>
+    <row r="402" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D402" s="5"/>
+    </row>
+    <row r="403" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D403" s="5"/>
+    </row>
+    <row r="404" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D404" s="5"/>
+    </row>
+    <row r="405" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D405" s="5"/>
+    </row>
+    <row r="406" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D406" s="5"/>
+    </row>
+    <row r="407" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D407" s="5"/>
+    </row>
+    <row r="408" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D408" s="5"/>
+    </row>
+    <row r="409" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D409" s="5"/>
+    </row>
+    <row r="410" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D410" s="5"/>
+    </row>
+    <row r="411" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D411" s="5"/>
+    </row>
+    <row r="412" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D412" s="5"/>
+    </row>
+    <row r="413" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D413" s="5"/>
+    </row>
+    <row r="414" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D414" s="5"/>
+    </row>
+    <row r="415" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D415" s="5"/>
+    </row>
+    <row r="416" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D416" s="5"/>
+    </row>
+    <row r="417" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D417" s="5"/>
+    </row>
+    <row r="418" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D418" s="5"/>
+    </row>
+    <row r="419" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D419" s="5"/>
+    </row>
+    <row r="420" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D420" s="5"/>
+    </row>
+    <row r="421" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D421" s="5"/>
+    </row>
+    <row r="422" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D422" s="5"/>
+    </row>
+    <row r="423" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D423" s="5"/>
+    </row>
+    <row r="424" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D424" s="5"/>
+    </row>
+    <row r="425" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D425" s="5"/>
+    </row>
+    <row r="426" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D426" s="5"/>
+    </row>
+    <row r="427" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D427" s="5"/>
+    </row>
+    <row r="428" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D428" s="5"/>
+    </row>
+    <row r="429" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D429" s="5"/>
+    </row>
+    <row r="430" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D430" s="5"/>
+    </row>
+    <row r="431" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D431" s="5"/>
+    </row>
+    <row r="432" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D432" s="5"/>
+    </row>
+    <row r="433" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D433" s="5"/>
+    </row>
+    <row r="434" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D434" s="5"/>
+    </row>
+    <row r="435" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D435" s="5"/>
+    </row>
+    <row r="436" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D436" s="5"/>
+    </row>
+    <row r="437" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D437" s="5"/>
+    </row>
+    <row r="438" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D438" s="5"/>
+    </row>
+    <row r="439" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D439" s="5"/>
+    </row>
+    <row r="440" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D440" s="5"/>
+    </row>
+    <row r="441" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D441" s="5"/>
+    </row>
+    <row r="442" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D442" s="5"/>
+    </row>
+    <row r="443" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D443" s="5"/>
+    </row>
+    <row r="444" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D444" s="5"/>
+    </row>
+    <row r="445" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D445" s="5"/>
+    </row>
+    <row r="446" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D446" s="5"/>
+    </row>
+    <row r="447" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D447" s="5"/>
+    </row>
+    <row r="448" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D448" s="5"/>
+    </row>
+    <row r="449" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D449" s="5"/>
+    </row>
+    <row r="450" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D450" s="5"/>
+    </row>
+    <row r="451" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D451" s="5"/>
+    </row>
+    <row r="452" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D452" s="5"/>
+    </row>
+    <row r="453" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D453" s="5"/>
+    </row>
+    <row r="454" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D454" s="5"/>
+    </row>
+    <row r="455" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D455" s="5"/>
+    </row>
+    <row r="456" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D456" s="5"/>
+    </row>
+    <row r="457" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D457" s="5"/>
+    </row>
+    <row r="458" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D458" s="5"/>
+    </row>
+    <row r="459" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D459" s="5"/>
+    </row>
+    <row r="460" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D460" s="5"/>
+    </row>
+    <row r="461" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D461" s="5"/>
+    </row>
+    <row r="462" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D462" s="5"/>
+    </row>
+    <row r="463" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D463" s="5"/>
+    </row>
+    <row r="464" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D464" s="5"/>
+    </row>
+    <row r="465" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D465" s="5"/>
+    </row>
+    <row r="466" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D466" s="5"/>
+    </row>
+    <row r="467" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D467" s="5"/>
+    </row>
+    <row r="468" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D468" s="5"/>
+    </row>
+    <row r="469" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D469" s="5"/>
+    </row>
+    <row r="470" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D470" s="5"/>
+    </row>
+    <row r="471" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D471" s="5"/>
+    </row>
+    <row r="472" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D472" s="5"/>
+    </row>
+    <row r="473" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D473" s="5"/>
+    </row>
+    <row r="474" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D474" s="5"/>
+    </row>
+    <row r="475" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D475" s="5"/>
+    </row>
+    <row r="476" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D476" s="5"/>
+    </row>
+    <row r="477" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D477" s="5"/>
+    </row>
+    <row r="478" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D478" s="5"/>
+    </row>
+    <row r="479" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D479" s="5"/>
+    </row>
+    <row r="480" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D480" s="5"/>
+    </row>
+    <row r="481" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D481" s="5"/>
+    </row>
+    <row r="482" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D482" s="5"/>
+    </row>
+    <row r="483" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D483" s="5"/>
+    </row>
+    <row r="484" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D484" s="5"/>
+    </row>
+    <row r="485" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D485" s="5"/>
+    </row>
+    <row r="486" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D486" s="5"/>
+    </row>
+    <row r="487" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D487" s="5"/>
+    </row>
+    <row r="488" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D488" s="5"/>
+    </row>
+    <row r="489" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D489" s="5"/>
+    </row>
+    <row r="490" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D490" s="5"/>
+    </row>
+    <row r="491" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D491" s="5"/>
+    </row>
+    <row r="492" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D492" s="5"/>
+    </row>
+    <row r="493" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D493" s="5"/>
+    </row>
+    <row r="494" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D494" s="5"/>
+    </row>
+    <row r="495" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D495" s="5"/>
+    </row>
+    <row r="496" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D496" s="5"/>
+    </row>
+    <row r="497" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D497" s="5"/>
+    </row>
+    <row r="498" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D498" s="5"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="K1:K1048576">
+    <cfRule type="containsText" dxfId="13" priority="1" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",K1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="2" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",K1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K498" xr:uid="{8B184686-23DD-4E58-859F-F0AF51B40202}">
+      <formula1>"Pass,Fail"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E498" xr:uid="{24D1D52A-8FC7-4057-A219-C32F47C9E685}">
+      <formula1>"GET,POST,DELETE,PUT,HEAD,OPTION"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add employee and user endpoints tests
</commit_message>
<xml_diff>
--- a/Documents/1_TestCases/TC03_API/TC03_API_TestCase.xlsx
+++ b/Documents/1_TestCases/TC03_API/TC03_API_TestCase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\Automation\OrangeHRM---Automation-Java-Playwright-JUnit-\Documents\1_TestCases\TC03_API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B08001-7425-41A8-AA36-8ED490CE29B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091B1C59-5515-4192-BB42-DB5F1EE44A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8115" yWindow="0" windowWidth="20685" windowHeight="15600" tabRatio="365" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="365" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="70">
   <si>
     <t>Test ID</t>
   </si>
@@ -314,6 +314,9 @@
   <si>
     <t>Requests should return 200
 Project should update with the new data</t>
+  </si>
+  <si>
+    <t>/api/v2/pim/employees/{id}</t>
   </si>
 </sst>
 </file>
@@ -410,70 +413,6 @@
   </cellStyles>
   <dxfs count="42">
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
@@ -532,6 +471,70 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -713,19 +716,19 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9C8EB052-938D-4D4D-B12E-C5AC8E21FC0E}" name="Table723" displayName="Table723" ref="B2:K498" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9C8EB052-938D-4D4D-B12E-C5AC8E21FC0E}" name="Table723" displayName="Table723" ref="B2:K498" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="B2:K498" xr:uid="{9C8EB052-938D-4D4D-B12E-C5AC8E21FC0E}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{8B447F5F-0218-44A8-9AD3-0BA2F0132139}" name="Test ID" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{D77FF6A0-CD02-4D99-8DEF-227253F4E9FC}" name="Description/Title" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{3B41C8A5-EB46-4059-8F73-33287EE9BE65}" name="Endpoint" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{B5E9853E-9C0B-477D-9161-7580076039E0}" name="Method" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{4D811123-D701-44EE-A284-D707FBE3753B}" name="Preconditions" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{489770C1-162F-420A-8DFC-5D079EA25964}" name="Test Steps" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{3D056CFF-89CB-412D-A5EB-A45D7A02B15B}" name="Expected Result" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{2765CC8E-9B99-450D-A70C-7EFAA02AF207}" name="Actual Result" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{C4579882-DBA1-426B-ABF8-139B3D94F8F2}" name="Notes" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{6F52D7A2-E330-4F92-AC74-2515DE0D07B1}" name="Status" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{8B447F5F-0218-44A8-9AD3-0BA2F0132139}" name="Test ID" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{D77FF6A0-CD02-4D99-8DEF-227253F4E9FC}" name="Description/Title" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{3B41C8A5-EB46-4059-8F73-33287EE9BE65}" name="Endpoint" dataDxfId="13"/>
+    <tableColumn id="11" xr3:uid="{B5E9853E-9C0B-477D-9161-7580076039E0}" name="Method" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{4D811123-D701-44EE-A284-D707FBE3753B}" name="Preconditions" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{489770C1-162F-420A-8DFC-5D079EA25964}" name="Test Steps" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{3D056CFF-89CB-412D-A5EB-A45D7A02B15B}" name="Expected Result" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{2765CC8E-9B99-450D-A70C-7EFAA02AF207}" name="Actual Result" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{C4579882-DBA1-426B-ABF8-139B3D94F8F2}" name="Notes" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{6F52D7A2-E330-4F92-AC74-2515DE0D07B1}" name="Status" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -997,7 +1000,7 @@
   <dimension ref="B2:K498"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,7 +1117,7 @@
         <v>25</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>26</v>
@@ -1127,6 +1130,9 @@
       </c>
       <c r="H5" s="3" t="s">
         <v>28</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="105" x14ac:dyDescent="0.25">
@@ -1151,6 +1157,9 @@
       <c r="H6" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="K6" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" s="5"/>
@@ -2631,10 +2640,10 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",K1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2658,8 +2667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F0733E0-18AD-4E8F-BD90-40A3BDD9A525}">
   <dimension ref="B2:K498"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2732,6 +2741,9 @@
       <c r="H3" s="3" t="s">
         <v>44</v>
       </c>
+      <c r="K3" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="4" spans="2:11" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
@@ -4280,10 +4292,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",K1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4306,7 +4318,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8267792D-E60E-4C51-8AAF-7230FC3414A8}">
   <dimension ref="B2:K498"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
@@ -5928,10 +5940,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="containsText" dxfId="13" priority="1" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",K1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="2" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",K1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add create user method and test
</commit_message>
<xml_diff>
--- a/Documents/1_TestCases/TC03_API/TC03_API_TestCase.xlsx
+++ b/Documents/1_TestCases/TC03_API/TC03_API_TestCase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\Automation\OrangeHRM---Automation-Java-Playwright-JUnit-\Documents\1_TestCases\TC03_API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091B1C59-5515-4192-BB42-DB5F1EE44A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048518A9-E326-4B20-A04A-6BDC23B9DBD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="365" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="71">
   <si>
     <t>Test ID</t>
   </si>
@@ -317,6 +317,9 @@
   </si>
   <si>
     <t>/api/v2/pim/employees/{id}</t>
+  </si>
+  <si>
+    <t>API_USER_TC03</t>
   </si>
 </sst>
 </file>
@@ -2668,7 +2671,7 @@
   <dimension ref="B2:K498"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2767,10 +2770,13 @@
       <c r="H4" s="3" t="s">
         <v>45</v>
       </c>
+      <c r="K4" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" spans="2:11" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
add delete/update user test cases, fixed password generation inconsistencies
</commit_message>
<xml_diff>
--- a/Documents/1_TestCases/TC03_API/TC03_API_TestCase.xlsx
+++ b/Documents/1_TestCases/TC03_API/TC03_API_TestCase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\Automation\OrangeHRM---Automation-Java-Playwright-JUnit-\Documents\1_TestCases\TC03_API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048518A9-E326-4B20-A04A-6BDC23B9DBD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C2F787-C350-46C3-988F-2EB1C158ED0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="365" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="71">
   <si>
     <t>Test ID</t>
   </si>
@@ -2671,7 +2671,7 @@
   <dimension ref="B2:K498"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2796,6 +2796,9 @@
       <c r="H5" s="3" t="s">
         <v>48</v>
       </c>
+      <c r="K5" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" spans="2:11" ht="120" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
@@ -2818,6 +2821,9 @@
       </c>
       <c r="H6" s="3" t="s">
         <v>50</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add update project test and updated docs
</commit_message>
<xml_diff>
--- a/Documents/1_TestCases/TC03_API/TC03_API_TestCase.xlsx
+++ b/Documents/1_TestCases/TC03_API/TC03_API_TestCase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\Automation\OrangeHRM---Automation-Java-Playwright-JUnit-\Documents\1_TestCases\TC03_API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C2F787-C350-46C3-988F-2EB1C158ED0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C356CBF-8EDD-4EE8-94AA-18F3828AEF09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="365" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="365" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="80">
   <si>
     <t>Test ID</t>
   </si>
@@ -261,72 +261,118 @@
 2.Verify project details</t>
   </si>
   <si>
-    <t>Details should match:
+    <t>Project details should match details added in the payload.</t>
+  </si>
+  <si>
+    <t>1.Send a DELETE request to endpoint with the following payload format:
+{
+  "ids": [1]
+}
+2.Verify request status.
+3.Send GET request to confirm project is not available anymore.</t>
+  </si>
+  <si>
+    <t>Delete request returns 200.
+Get request return 40X
+Project is not available.</t>
+  </si>
+  <si>
+    <t>1.Send a GET request to endpoint with {id} = 2 to retrieve info about project.
+2.Send a PUT request to endpoint with a format similar to API_PROJECTS_TC02 and with new data.
+3.Send a GET request to endpoint with {id} = 2 to retrieve info about project and cofirm the update has been succesfull.</t>
+  </si>
+  <si>
+    <t>Requests should return 200
+Project should update with the new data</t>
+  </si>
+  <si>
+    <t>/api/v2/pim/employees/{id}</t>
+  </si>
+  <si>
+    <t>API_USER_TC03</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">/api/v2/time/projects/{id}
+OR
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>/api/v2/time/projects/{id}?model=detailed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Details should match:
 Name: Automation Project
 Description: Automation Project
-Customer Name: OrangeHRM
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Customer Name: OrangeHRM
 Project Admin: Mary Great</t>
-  </si>
-  <si>
-    <t>Project details should match details added in the payload.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1.Send a POST request to endpoint with the following payload format:
+    </r>
+  </si>
+  <si>
+    <t>1.Send a POST request to endpoint with the following payload format:
 {
   "customerId": 1,
   "name": "projectName",
   "description": "projectDescription",
   "projectAdminsEmpNumbers": [1]
 }
-2.Verify project request status and GET project details to confirm creation. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Response may not include details)</t>
-    </r>
-  </si>
-  <si>
-    <t>1.Send a DELETE request to endpoint with the following payload format:
-{
-  "ids": [1]
-}
-2.Verify request status.
-3.Send GET request to confirm project is not available anymore.</t>
-  </si>
-  <si>
-    <t>Delete request returns 200.
-Get request return 40X
-Project is not available.</t>
-  </si>
-  <si>
-    <t>1.Send a GET request to endpoint with {id} = 2 to retrieve info about project.
-2.Send a PUT request to endpoint with a format similar to API_PROJECTS_TC02 and with new data.
-3.Send a GET request to endpoint with {id} = 2 to retrieve info about project and cofirm the update has been succesfull.</t>
-  </si>
-  <si>
-    <t>Requests should return 200
-Project should update with the new data</t>
-  </si>
-  <si>
-    <t>/api/v2/pim/employees/{id}</t>
-  </si>
-  <si>
-    <t>API_USER_TC03</t>
+2.Verify project response status and GET project details to confirm creation.</t>
+  </si>
+  <si>
+    <t>Status 200
+Values match</t>
+  </si>
+  <si>
+    <t>Status 200
+Project created with desired values</t>
+  </si>
+  <si>
+    <t>Status 200
+Project updated with correct values</t>
+  </si>
+  <si>
+    <t>Status 200
+User is created with correct values</t>
+  </si>
+  <si>
+    <t>Status 200
+User is deleted,</t>
+  </si>
+  <si>
+    <t>Status 200
+User is updated with desired values</t>
+  </si>
+  <si>
+    <t>Status 200
+Count value is correct</t>
+  </si>
+  <si>
+    <t>Unless "?model=detailed" is added to endpoint, Customer Name and Project Admin elements won't be available in response.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,9 +408,14 @@
       <family val="3"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1003,7 +1054,7 @@
   <dimension ref="B2:K498"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1120,7 +1171,7 @@
         <v>25</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>26</v>
@@ -1133,6 +1184,9 @@
       </c>
       <c r="H5" s="3" t="s">
         <v>28</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>19</v>
@@ -1159,6 +1213,9 @@
       </c>
       <c r="H6" s="3" t="s">
         <v>18</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>19</v>
@@ -2670,8 +2727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F0733E0-18AD-4E8F-BD90-40A3BDD9A525}">
   <dimension ref="B2:K498"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2744,6 +2801,9 @@
       <c r="H3" s="3" t="s">
         <v>44</v>
       </c>
+      <c r="I3" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="K3" s="4" t="s">
         <v>19</v>
       </c>
@@ -2770,13 +2830,16 @@
       <c r="H4" s="3" t="s">
         <v>45</v>
       </c>
+      <c r="I4" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="K4" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>39</v>
@@ -2795,6 +2858,9 @@
       </c>
       <c r="H5" s="3" t="s">
         <v>48</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>19</v>
@@ -2821,6 +2887,9 @@
       </c>
       <c r="H6" s="3" t="s">
         <v>50</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>19</v>
@@ -4330,8 +4399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8267792D-E60E-4C51-8AAF-7230FC3414A8}">
   <dimension ref="B2:K498"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4382,7 +4451,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" ht="90" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>51</v>
       </c>
@@ -4390,7 +4459,7 @@
         <v>56</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>26</v>
@@ -4402,10 +4471,19 @@
         <v>61</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" ht="180" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="165" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>52</v>
       </c>
@@ -4422,10 +4500,16 @@
         <v>17</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="120" x14ac:dyDescent="0.25">
@@ -4445,10 +4529,16 @@
         <v>17</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="165" x14ac:dyDescent="0.25">
@@ -4468,10 +4558,16 @@
         <v>17</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>